<commit_message>
DB Location table changes; Updated IVLP Load SSIS packages
</commit_message>
<xml_diff>
--- a/App/ECA.Database/Data Migration/Sample Data/ECA/Country XREF ISO FIPS.xlsx
+++ b/App/ECA.Database/Data Migration/Sample Data/ECA/Country XREF ISO FIPS.xlsx
@@ -3922,10 +3922,13 @@
   <dimension ref="A1:I253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3985,7 +3988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
@@ -4014,7 +4017,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -4043,7 +4046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -4072,7 +4075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -4159,7 +4162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
@@ -4215,7 +4218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -4242,7 +4245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -4271,7 +4274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -5104,7 +5107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>179</v>
       </c>
@@ -6755,7 +6758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>421</v>
       </c>
@@ -7043,7 +7046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>464</v>
       </c>
@@ -10836,7 +10839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>1016</v>
       </c>

</xml_diff>